<commit_message>
The robot is now capable of following the line! Hooray!
</commit_message>
<xml_diff>
--- a/IR sensor outputs.xlsx
+++ b/IR sensor outputs.xlsx
@@ -3482,8 +3482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932958A4-F64A-4305-9564-56C90EC136CD}">
   <dimension ref="A1:T175"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+    <sheetView topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="L116" sqref="L116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9929,8 +9929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E03C2029-D67C-49CA-8646-65AC2878C8D2}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:P4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>